<commit_message>
new format and data added
</commit_message>
<xml_diff>
--- a/college.xlsx
+++ b/college.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="60">
   <si>
     <t>level0</t>
   </si>
@@ -82,18 +82,9 @@
     <t>Engineering exams</t>
   </si>
   <si>
-    <t>GRE</t>
-  </si>
-  <si>
-    <t>TOEFL</t>
-  </si>
-  <si>
     <t>Marathi</t>
   </si>
   <si>
-    <t>form_field</t>
-  </si>
-  <si>
     <t>Hindi</t>
   </si>
   <si>
@@ -160,21 +151,6 @@
     <t>semester 8</t>
   </si>
   <si>
-    <t>GATE</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>Electrical Engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronics and Communication Engineering </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mechanical Engineering </t>
-  </si>
-  <si>
     <t>Morning</t>
   </si>
   <si>
@@ -184,10 +160,40 @@
     <t>Evening</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Technical</t>
+    <t>Final Exam</t>
+  </si>
+  <si>
+    <t>Practice Exam</t>
+  </si>
+  <si>
+    <t>GRE for Engineering</t>
+  </si>
+  <si>
+    <t>GRE for Pharmacy</t>
+  </si>
+  <si>
+    <t>GRE final</t>
+  </si>
+  <si>
+    <t>TOEFL  final</t>
+  </si>
+  <si>
+    <t>GATE  final</t>
+  </si>
+  <si>
+    <t>GRE practice</t>
+  </si>
+  <si>
+    <t>TOEFL practice</t>
+  </si>
+  <si>
+    <t>GATE practice</t>
+  </si>
+  <si>
+    <t>GATE final list</t>
+  </si>
+  <si>
+    <t>GATE practice list</t>
   </si>
 </sst>
 </file>
@@ -1009,18 +1015,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1153,7 +1162,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" ref="B12:B20" si="0">LOOKUP(C12,$C$3:$C$7,$A$3:$A$7)</f>
+        <f t="shared" ref="B12:B19" si="0">LOOKUP(C12,$C$3:$C$7,$A$3:$A$7)</f>
         <v>primary</v>
       </c>
       <c r="C12">
@@ -1167,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" ref="F12:F20" si="1">IF(E12&lt;&gt;1,"level2","form_field")</f>
+        <f t="shared" ref="F12:F19" si="1">IF(E12&lt;&gt;1,"level2","form_field")</f>
         <v>level2</v>
       </c>
     </row>
@@ -1183,7 +1192,7 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:D20" si="2">IF(C13&lt;&gt;C12,((C13*100)+1),(D12+1))</f>
+        <f t="shared" ref="D13:D19" si="2">IF(C13&lt;&gt;C12,((C13*100)+1),(D12+1))</f>
         <v>103</v>
       </c>
       <c r="E13">
@@ -1288,7 +1297,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -1311,7 +1320,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -1332,702 +1341,679 @@
         <v>level2</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>comp</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>503</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="1"/>
-        <v>level2</v>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="B23" t="str">
+        <f>LOOKUP(C23,$D$11:$D$19,$A$11:$A$19)</f>
+        <v>SSC</v>
+      </c>
+      <c r="C23">
+        <v>101</v>
+      </c>
+      <c r="D23">
+        <v>10101</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="str">
+        <f>IF(E23&lt;&gt;1,"level3","form_field")</f>
+        <v>form_field</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="str">
-        <f>LOOKUP(C24,$D$11:$D$20,$A$11:$A$20)</f>
+        <f>LOOKUP(C24,$D$11:$D$19,$A$11:$A$19)</f>
         <v>SSC</v>
       </c>
       <c r="C24">
         <v>101</v>
       </c>
       <c r="D24">
-        <v>10101</v>
+        <f>IF(C24&lt;&gt;C23,((C24*100)+1),(D23+1))</f>
+        <v>10102</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="str">
-        <f>IF(E24&lt;&gt;1,"level3","form_field")</f>
+        <f t="shared" ref="F24:F39" si="3">IF(E24&lt;&gt;1,"level3","form_field")</f>
         <v>form_field</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" ref="B25:B40" si="3">LOOKUP(C25,$D$11:$D$20,$A$11:$A$20)</f>
+        <f>LOOKUP(C25,$D$11:$D$19,$A$11:$A$19)</f>
         <v>SSC</v>
       </c>
       <c r="C25">
         <v>101</v>
       </c>
       <c r="D25">
-        <f>IF(C25&lt;&gt;C24,((C25*100)+1),(D24+1))</f>
-        <v>10102</v>
+        <f t="shared" ref="D25:D39" si="4">IF(C25&lt;&gt;C24,((C25*100)+1),(D24+1))</f>
+        <v>10103</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" ref="F25:F40" si="4">IF(E25&lt;&gt;1,"level3","form_field")</f>
+        <f t="shared" si="3"/>
         <v>form_field</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="3"/>
+        <f>LOOKUP(C26,$D$11:$D$19,$A$11:$A$19)</f>
         <v>SSC</v>
       </c>
       <c r="C26">
         <v>101</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:D40" si="5">IF(C26&lt;&gt;C25,((C26*100)+1),(D25+1))</f>
-        <v>10103</v>
+        <f t="shared" si="4"/>
+        <v>10104</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>form_field</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" t="str">
+        <f>LOOKUP(C27,$D$11:$D$19,$A$11:$A$19)</f>
+        <v>HSC</v>
+      </c>
+      <c r="C27">
+        <v>202</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="4"/>
+        <v>20201</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="str">
         <f t="shared" si="3"/>
-        <v>SSC</v>
-      </c>
-      <c r="C27">
-        <v>101</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="5"/>
-        <v>10104</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" t="str">
-        <f t="shared" si="4"/>
-        <v>form_field</v>
+        <v>level3</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="3"/>
+        <f>LOOKUP(C28,$D$11:$D$19,$A$11:$A$19)</f>
         <v>HSC</v>
       </c>
       <c r="C28">
         <v>202</v>
       </c>
       <c r="D28">
-        <f t="shared" si="5"/>
-        <v>20201</v>
+        <f t="shared" si="4"/>
+        <v>20202</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>level3</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="3"/>
+        <f>LOOKUP(C29,$D$11:$D$19,$A$11:$A$19)</f>
         <v>HSC</v>
       </c>
       <c r="C29">
         <v>202</v>
       </c>
       <c r="D29">
-        <f t="shared" si="5"/>
-        <v>20202</v>
+        <f t="shared" si="4"/>
+        <v>20203</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>level3</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="3"/>
-        <v>HSC</v>
+        <f>LOOKUP(C30,$D$11:$D$19,$A$11:$A$19)</f>
+        <v>Engineering exams</v>
       </c>
       <c r="C30">
-        <v>202</v>
+        <v>301</v>
       </c>
       <c r="D30">
-        <f t="shared" si="5"/>
-        <v>20203</v>
+        <f t="shared" si="4"/>
+        <v>30101</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>level3</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="3"/>
+        <f>LOOKUP(C31,$D$11:$D$19,$A$11:$A$19)</f>
         <v>Engineering exams</v>
       </c>
       <c r="C31">
         <v>301</v>
       </c>
       <c r="D31">
-        <f t="shared" si="5"/>
-        <v>30101</v>
+        <f t="shared" si="4"/>
+        <v>30102</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>level3</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="3"/>
+        <f>LOOKUP(C32,$D$11:$D$19,$A$11:$A$19)</f>
         <v>Engineering exams</v>
       </c>
       <c r="C32">
         <v>301</v>
       </c>
       <c r="D32">
-        <f t="shared" si="5"/>
-        <v>30102</v>
+        <f t="shared" si="4"/>
+        <v>30103</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>level3</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="3"/>
+        <f>LOOKUP(C33,$D$11:$D$19,$A$11:$A$19)</f>
         <v>Engineering exams</v>
       </c>
       <c r="C33">
         <v>301</v>
       </c>
       <c r="D33">
-        <f t="shared" si="5"/>
-        <v>30103</v>
+        <f t="shared" si="4"/>
+        <v>30104</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>level3</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="3"/>
-        <v>Engineering exams</v>
+        <f>LOOKUP(C34,$D$11:$D$19,$A$11:$A$19)</f>
+        <v>Final Exam</v>
       </c>
       <c r="C34">
-        <v>301</v>
+        <v>501</v>
       </c>
       <c r="D34">
-        <f t="shared" si="5"/>
-        <v>30104</v>
+        <f t="shared" si="4"/>
+        <v>50101</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>level3</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B35" t="str">
-        <f>LOOKUP(C35,$D$11:$D$20,$A$11:$A$20)</f>
-        <v>GRE</v>
+        <f>LOOKUP(C35,$D$11:$D$19,$A$11:$A$19)</f>
+        <v>Final Exam</v>
       </c>
       <c r="C35">
         <v>501</v>
       </c>
       <c r="D35">
-        <f t="shared" si="5"/>
-        <v>50101</v>
+        <f t="shared" si="4"/>
+        <v>50102</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="4"/>
-        <v>level3</v>
+        <f t="shared" si="3"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="3"/>
-        <v>GRE</v>
+        <f>LOOKUP(C36,$D$11:$D$19,$A$11:$A$19)</f>
+        <v>Final Exam</v>
       </c>
       <c r="C36">
         <v>501</v>
       </c>
       <c r="D36">
-        <f t="shared" si="5"/>
-        <v>50102</v>
+        <f t="shared" si="4"/>
+        <v>50103</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>level3</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B37" t="str">
+        <f>LOOKUP(C37,$D$11:$D$19,$A$11:$A$19)</f>
+        <v>Practice Exam</v>
+      </c>
+      <c r="C37">
+        <v>502</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="4"/>
+        <v>50201</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="str">
         <f t="shared" si="3"/>
-        <v>GATE</v>
-      </c>
-      <c r="C37">
-        <v>503</v>
-      </c>
-      <c r="D37">
-        <f>IF(C37&lt;&gt;C34,((C37*100)+1),(D34+1))</f>
-        <v>50301</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37" t="str">
-        <f t="shared" si="4"/>
-        <v>form_field</v>
+        <v>level3</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B38" t="str">
+        <f>LOOKUP(C38,$D$11:$D$19,$A$11:$A$19)</f>
+        <v>Practice Exam</v>
+      </c>
+      <c r="C38">
+        <v>502</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="4"/>
+        <v>50202</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="str">
         <f t="shared" si="3"/>
-        <v>GATE</v>
-      </c>
-      <c r="C38">
-        <v>503</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="5"/>
-        <v>50302</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38" t="str">
-        <f t="shared" si="4"/>
         <v>form_field</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B39" t="str">
+        <f>LOOKUP(C39,$D$11:$D$19,$A$11:$A$19)</f>
+        <v>Practice Exam</v>
+      </c>
+      <c r="C39">
+        <v>502</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="4"/>
+        <v>50203</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="str">
         <f t="shared" si="3"/>
-        <v>GATE</v>
-      </c>
-      <c r="C39">
-        <v>503</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="5"/>
-        <v>50303</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" t="str">
-        <f t="shared" si="4"/>
-        <v>form_field</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" t="str">
-        <f t="shared" si="3"/>
-        <v>GATE</v>
-      </c>
-      <c r="C40">
-        <v>503</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="5"/>
-        <v>50304</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40" t="str">
-        <f t="shared" si="4"/>
-        <v>form_field</v>
+        <v>level3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" t="s">
-        <v>14</v>
+        <v>34</v>
+      </c>
+      <c r="B43" t="str">
+        <f>LOOKUP(C43,$D$23:$D$39,$A$23:$A$39)</f>
+        <v>Information Technology</v>
+      </c>
+      <c r="C43">
+        <v>30101</v>
+      </c>
+      <c r="D43">
+        <f>C43*100+1</f>
+        <v>3010101</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="str">
+        <f>IF(E43&lt;&gt;1,"level4","form_field")</f>
+        <v>level4</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B44" t="str">
-        <f>LOOKUP(C44,$D$24:$D$40,$A$24:$A$40)</f>
-        <v>Information Technology</v>
+        <f>LOOKUP(C44,$D$23:$D$39,$A$23:$A$39)</f>
+        <v>Computer Engineering</v>
       </c>
       <c r="C44">
-        <v>30101</v>
+        <v>30102</v>
       </c>
       <c r="D44">
-        <f>C44*100+1</f>
-        <v>3010101</v>
+        <f>IF(C44&lt;&gt;C43,((C44*100)+1),(D43+1))</f>
+        <v>3010201</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44" t="str">
-        <f>IF(E44&lt;&gt;1,"level4","form_field")</f>
+        <f t="shared" ref="F44:F52" si="5">IF(E44&lt;&gt;1,"level4","form_field")</f>
         <v>level4</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" ref="B45:B53" si="6">LOOKUP(C45,$D$24:$D$40,$A$24:$A$40)</f>
-        <v>Computer Engineering</v>
+        <f t="shared" ref="B44:B52" si="6">LOOKUP(C45,$D$23:$D$39,$A$23:$A$39)</f>
+        <v>Electronic Engineering</v>
       </c>
       <c r="C45">
-        <v>30102</v>
+        <v>30103</v>
       </c>
       <c r="D45">
-        <f>IF(C45&lt;&gt;C44,((C45*100)+1),(D44+1))</f>
-        <v>3010201</v>
+        <f t="shared" ref="D45:D52" si="7">IF(C45&lt;&gt;C44,((C45*100)+1),(D44+1))</f>
+        <v>3010301</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" ref="F45:F53" si="7">IF(E45&lt;&gt;1,"level4","form_field")</f>
+        <f t="shared" si="5"/>
         <v>level4</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="6"/>
-        <v>Electronic Engineering</v>
+        <v>electronic &amp; Telecommunication</v>
       </c>
       <c r="C46">
-        <v>30103</v>
+        <v>30104</v>
       </c>
       <c r="D46">
-        <f t="shared" ref="D46:D53" si="8">IF(C46&lt;&gt;C45,((C46*100)+1),(D45+1))</f>
-        <v>3010301</v>
+        <f t="shared" si="7"/>
+        <v>3010401</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>level4</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="6"/>
-        <v>electronic &amp; Telecommunication</v>
+        <v>GRE final</v>
       </c>
       <c r="C47">
-        <v>30104</v>
+        <v>50101</v>
       </c>
       <c r="D47">
-        <f t="shared" si="8"/>
-        <v>3010401</v>
+        <f t="shared" si="7"/>
+        <v>5010101</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="7"/>
-        <v>level4</v>
+        <f t="shared" si="5"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="6"/>
-        <v>Normal</v>
+        <v>GRE final</v>
       </c>
       <c r="C48">
         <v>50101</v>
       </c>
       <c r="D48">
-        <f t="shared" si="8"/>
-        <v>5010101</v>
+        <f t="shared" si="7"/>
+        <v>5010102</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>form_field</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="6"/>
-        <v>Normal</v>
+        <v>GATE  final</v>
       </c>
       <c r="C49">
-        <v>50101</v>
+        <v>50103</v>
       </c>
       <c r="D49">
-        <f t="shared" si="8"/>
-        <v>5010102</v>
+        <f t="shared" si="7"/>
+        <v>5010301</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="7"/>
-        <v>form_field</v>
+        <f t="shared" si="5"/>
+        <v>level4</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="6"/>
-        <v>Normal</v>
+        <v>GATE practice</v>
       </c>
       <c r="C50">
-        <v>50101</v>
+        <v>50203</v>
       </c>
       <c r="D50">
-        <f t="shared" si="8"/>
-        <v>5010103</v>
+        <f t="shared" si="7"/>
+        <v>5020301</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="7"/>
-        <v>form_field</v>
+        <f t="shared" si="5"/>
+        <v>level4</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="6"/>
-        <v>Technical</v>
+        <v>GRE practice</v>
       </c>
       <c r="C51">
-        <v>50102</v>
+        <v>50201</v>
       </c>
       <c r="D51">
-        <f t="shared" si="8"/>
-        <v>5010201</v>
+        <f>IF(C51&lt;&gt;C48,((C51*100)+1),(D48+1))</f>
+        <v>5020101</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>form_field</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="6"/>
-        <v>Technical</v>
+        <v>GRE practice</v>
       </c>
       <c r="C52">
-        <v>50102</v>
+        <v>50201</v>
       </c>
       <c r="D52">
-        <f t="shared" si="8"/>
-        <v>5010202</v>
+        <f>IF(C52&lt;&gt;C51,((C52*100)+1),(D51+1))</f>
+        <v>5020102</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="7"/>
-        <v>form_field</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" t="str">
-        <f t="shared" si="6"/>
-        <v>Technical</v>
-      </c>
-      <c r="C53">
-        <v>50102</v>
-      </c>
-      <c r="D53">
-        <f t="shared" si="8"/>
-        <v>5010203</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53" t="str">
-        <f t="shared" si="7"/>
-        <v>form_field</v>
+        <f t="shared" si="5"/>
+        <v>level4</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2038,7 +2024,7 @@
         <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -2055,13 +2041,14 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>40</v>
-      </c>
-      <c r="B57" t="s">
         <v>37</v>
       </c>
+      <c r="B57" t="str">
+        <f>LOOKUP(D57,$D$43:$D$52,$A$43:$A$52)</f>
+        <v>Mumbai University</v>
+      </c>
       <c r="C57" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D57">
         <v>3010101</v>
@@ -2072,721 +2059,977 @@
       <c r="F57">
         <v>1</v>
       </c>
-      <c r="G57" t="s">
-        <v>25</v>
+      <c r="G57" t="str">
+        <f>IF(F57&lt;&gt;1,"level5","form_field")</f>
+        <v>form_field</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>41</v>
-      </c>
-      <c r="B58" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" ref="B58:B94" si="8">LOOKUP(D58,$D$43:$D$52,$A$43:$A$52)</f>
+        <v>Mumbai University</v>
       </c>
       <c r="C58" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D58">
         <v>3010101</v>
       </c>
       <c r="E58">
+        <f>IF(D58&lt;&gt;D57,((D58*100)+1),(E57+1))</f>
         <v>301010102</v>
       </c>
       <c r="F58">
         <v>1</v>
       </c>
-      <c r="G58" t="s">
-        <v>25</v>
+      <c r="G58" t="str">
+        <f t="shared" ref="G58:G94" si="9">IF(F58&lt;&gt;1,"level5","form_field")</f>
+        <v>form_field</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B59" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C59" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D59">
         <v>3010101</v>
       </c>
       <c r="E59">
+        <f t="shared" ref="E59:E95" si="10">IF(D59&lt;&gt;D58,((D59*100)+1),(E58+1))</f>
         <v>301010103</v>
       </c>
       <c r="F59">
         <v>1</v>
       </c>
-      <c r="G59" t="s">
-        <v>25</v>
+      <c r="G59" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>43</v>
-      </c>
-      <c r="B60" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C60" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D60">
         <v>3010101</v>
       </c>
       <c r="E60">
+        <f t="shared" si="10"/>
         <v>301010104</v>
       </c>
       <c r="F60">
         <v>1</v>
       </c>
-      <c r="G60" t="s">
-        <v>25</v>
+      <c r="G60" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>44</v>
-      </c>
-      <c r="B61" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C61" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D61">
         <v>3010101</v>
       </c>
       <c r="E61">
+        <f t="shared" si="10"/>
         <v>301010105</v>
       </c>
       <c r="F61">
         <v>1</v>
       </c>
-      <c r="G61" t="s">
-        <v>25</v>
+      <c r="G61" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>45</v>
-      </c>
-      <c r="B62" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C62" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D62">
         <v>3010101</v>
       </c>
       <c r="E62">
+        <f t="shared" si="10"/>
         <v>301010106</v>
       </c>
       <c r="F62">
         <v>1</v>
       </c>
-      <c r="G62" t="s">
-        <v>25</v>
+      <c r="G62" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>46</v>
-      </c>
-      <c r="B63" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C63" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D63">
         <v>3010101</v>
       </c>
       <c r="E63">
+        <f t="shared" si="10"/>
         <v>301010107</v>
       </c>
       <c r="F63">
         <v>1</v>
       </c>
-      <c r="G63" t="s">
-        <v>25</v>
+      <c r="G63" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>47</v>
-      </c>
-      <c r="B64" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C64" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D64">
         <v>3010101</v>
       </c>
       <c r="E64">
+        <f t="shared" si="10"/>
         <v>301010108</v>
       </c>
       <c r="F64">
         <v>1</v>
       </c>
-      <c r="G64" t="s">
-        <v>25</v>
+      <c r="G64" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>40</v>
-      </c>
-      <c r="B65" t="s">
         <v>37</v>
       </c>
+      <c r="B65" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
+      </c>
       <c r="C65" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D65">
         <v>3010201</v>
       </c>
       <c r="E65">
+        <f t="shared" si="10"/>
         <v>301020101</v>
       </c>
       <c r="F65">
         <v>1</v>
       </c>
-      <c r="G65" t="s">
-        <v>25</v>
+      <c r="G65" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>41</v>
-      </c>
-      <c r="B66" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C66" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D66">
         <v>3010201</v>
       </c>
       <c r="E66">
+        <f t="shared" si="10"/>
         <v>301020102</v>
       </c>
       <c r="F66">
         <v>1</v>
       </c>
-      <c r="G66" t="s">
-        <v>25</v>
+      <c r="G66" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>42</v>
-      </c>
-      <c r="B67" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C67" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D67">
         <v>3010201</v>
       </c>
       <c r="E67">
+        <f t="shared" si="10"/>
         <v>301020103</v>
       </c>
       <c r="F67">
         <v>1</v>
       </c>
-      <c r="G67" t="s">
-        <v>25</v>
+      <c r="G67" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>43</v>
-      </c>
-      <c r="B68" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C68" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D68">
         <v>3010201</v>
       </c>
       <c r="E68">
+        <f t="shared" si="10"/>
         <v>301020104</v>
       </c>
       <c r="F68">
         <v>1</v>
       </c>
-      <c r="G68" t="s">
-        <v>25</v>
+      <c r="G68" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>44</v>
-      </c>
-      <c r="B69" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C69" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D69">
         <v>3010201</v>
       </c>
       <c r="E69">
+        <f t="shared" si="10"/>
         <v>301020105</v>
       </c>
       <c r="F69">
         <v>1</v>
       </c>
-      <c r="G69" t="s">
-        <v>25</v>
+      <c r="G69" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>45</v>
-      </c>
-      <c r="B70" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C70" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D70">
         <v>3010201</v>
       </c>
       <c r="E70">
+        <f t="shared" si="10"/>
         <v>301020106</v>
       </c>
       <c r="F70">
         <v>1</v>
       </c>
-      <c r="G70" t="s">
-        <v>25</v>
+      <c r="G70" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>46</v>
-      </c>
-      <c r="B71" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C71" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D71">
         <v>3010201</v>
       </c>
       <c r="E71">
+        <f t="shared" si="10"/>
         <v>301020107</v>
       </c>
       <c r="F71">
         <v>1</v>
       </c>
-      <c r="G71" t="s">
-        <v>25</v>
+      <c r="G71" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>47</v>
-      </c>
-      <c r="B72" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C72" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D72">
         <v>3010201</v>
       </c>
       <c r="E72">
+        <f t="shared" si="10"/>
         <v>301020108</v>
       </c>
       <c r="F72">
         <v>1</v>
       </c>
-      <c r="G72" t="s">
-        <v>25</v>
+      <c r="G72" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>40</v>
-      </c>
-      <c r="B73" t="s">
         <v>37</v>
       </c>
+      <c r="B73" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
+      </c>
       <c r="C73" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D73">
         <v>3010301</v>
       </c>
       <c r="E73">
+        <f t="shared" si="10"/>
         <v>301030101</v>
       </c>
       <c r="F73">
         <v>1</v>
       </c>
-      <c r="G73" t="s">
-        <v>25</v>
+      <c r="G73" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>41</v>
-      </c>
-      <c r="B74" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C74" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D74">
         <v>3010301</v>
       </c>
       <c r="E74">
+        <f t="shared" si="10"/>
         <v>301030102</v>
       </c>
       <c r="F74">
         <v>1</v>
       </c>
-      <c r="G74" t="s">
-        <v>25</v>
+      <c r="G74" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>42</v>
-      </c>
-      <c r="B75" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C75" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D75">
         <v>3010301</v>
       </c>
       <c r="E75">
+        <f t="shared" si="10"/>
         <v>301030103</v>
       </c>
       <c r="F75">
         <v>1</v>
       </c>
-      <c r="G75" t="s">
-        <v>25</v>
+      <c r="G75" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>43</v>
-      </c>
-      <c r="B76" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C76" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D76">
         <v>3010301</v>
       </c>
       <c r="E76">
+        <f t="shared" si="10"/>
         <v>301030104</v>
       </c>
       <c r="F76">
         <v>1</v>
       </c>
-      <c r="G76" t="s">
-        <v>25</v>
+      <c r="G76" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>44</v>
-      </c>
-      <c r="B77" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C77" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D77">
         <v>3010301</v>
       </c>
       <c r="E77">
+        <f t="shared" si="10"/>
         <v>301030105</v>
       </c>
       <c r="F77">
         <v>1</v>
       </c>
-      <c r="G77" t="s">
-        <v>25</v>
+      <c r="G77" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>45</v>
-      </c>
-      <c r="B78" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C78" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D78">
         <v>3010301</v>
       </c>
       <c r="E78">
+        <f t="shared" si="10"/>
         <v>301030106</v>
       </c>
       <c r="F78">
         <v>1</v>
       </c>
-      <c r="G78" t="s">
-        <v>25</v>
+      <c r="G78" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>46</v>
-      </c>
-      <c r="B79" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C79" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D79">
         <v>3010301</v>
       </c>
       <c r="E79">
+        <f t="shared" si="10"/>
         <v>301030107</v>
       </c>
       <c r="F79">
         <v>1</v>
       </c>
-      <c r="G79" t="s">
-        <v>25</v>
+      <c r="G79" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>47</v>
-      </c>
-      <c r="B80" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C80" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D80">
         <v>3010301</v>
       </c>
       <c r="E80">
+        <f t="shared" si="10"/>
         <v>301030108</v>
       </c>
       <c r="F80">
         <v>1</v>
       </c>
-      <c r="G80" t="s">
-        <v>25</v>
+      <c r="G80" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>40</v>
-      </c>
-      <c r="B81" t="s">
         <v>37</v>
       </c>
+      <c r="B81" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
+      </c>
       <c r="C81" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D81">
         <v>3010401</v>
       </c>
       <c r="E81">
+        <f t="shared" si="10"/>
         <v>301040101</v>
       </c>
       <c r="F81">
         <v>1</v>
       </c>
-      <c r="G81" t="s">
-        <v>25</v>
+      <c r="G81" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>41</v>
-      </c>
-      <c r="B82" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C82" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D82">
         <v>3010401</v>
       </c>
       <c r="E82">
+        <f t="shared" si="10"/>
         <v>301040102</v>
       </c>
       <c r="F82">
         <v>1</v>
       </c>
-      <c r="G82" t="s">
-        <v>25</v>
+      <c r="G82" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>42</v>
-      </c>
-      <c r="B83" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C83" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D83">
         <v>3010401</v>
       </c>
       <c r="E83">
+        <f t="shared" si="10"/>
         <v>301040103</v>
       </c>
       <c r="F83">
         <v>1</v>
       </c>
-      <c r="G83" t="s">
-        <v>25</v>
+      <c r="G83" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>43</v>
-      </c>
-      <c r="B84" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C84" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D84">
         <v>3010401</v>
       </c>
       <c r="E84">
+        <f t="shared" si="10"/>
         <v>301040104</v>
       </c>
       <c r="F84">
         <v>1</v>
       </c>
-      <c r="G84" t="s">
-        <v>25</v>
+      <c r="G84" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>44</v>
-      </c>
-      <c r="B85" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B85" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C85" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D85">
         <v>3010401</v>
       </c>
       <c r="E85">
+        <f t="shared" si="10"/>
         <v>301040105</v>
       </c>
       <c r="F85">
         <v>1</v>
       </c>
-      <c r="G85" t="s">
-        <v>25</v>
+      <c r="G85" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>45</v>
-      </c>
-      <c r="B86" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="B86" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C86" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D86">
         <v>3010401</v>
       </c>
       <c r="E86">
+        <f t="shared" si="10"/>
         <v>301040106</v>
       </c>
       <c r="F86">
         <v>1</v>
       </c>
-      <c r="G86" t="s">
-        <v>25</v>
+      <c r="G86" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>46</v>
-      </c>
-      <c r="B87" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="B87" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C87" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D87">
         <v>3010401</v>
       </c>
       <c r="E87">
+        <f t="shared" si="10"/>
         <v>301040107</v>
       </c>
       <c r="F87">
         <v>1</v>
       </c>
-      <c r="G87" t="s">
-        <v>25</v>
+      <c r="G87" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>47</v>
-      </c>
-      <c r="B88" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="B88" t="str">
+        <f t="shared" si="8"/>
+        <v>Mumbai University</v>
       </c>
       <c r="C88" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D88">
         <v>3010401</v>
       </c>
       <c r="E88">
+        <f t="shared" si="10"/>
         <v>301040108</v>
       </c>
       <c r="F88">
         <v>1</v>
       </c>
-      <c r="G88" t="s">
-        <v>25</v>
+      <c r="G88" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>45</v>
+      </c>
+      <c r="B89" t="str">
+        <f t="shared" si="8"/>
+        <v>GRE for Engineering</v>
+      </c>
+      <c r="C89" t="s">
+        <v>33</v>
+      </c>
+      <c r="D89">
+        <v>5010101</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="10"/>
+        <v>501010101</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>46</v>
+      </c>
+      <c r="B90" t="str">
+        <f t="shared" si="8"/>
+        <v>GRE for Engineering</v>
+      </c>
+      <c r="C90" t="s">
+        <v>33</v>
+      </c>
+      <c r="D90">
+        <v>5010101</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="10"/>
+        <v>501010102</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>47</v>
+      </c>
+      <c r="B91" t="str">
+        <f t="shared" si="8"/>
+        <v>GRE for Engineering</v>
+      </c>
+      <c r="C91" t="s">
+        <v>33</v>
+      </c>
+      <c r="D91">
+        <v>5010101</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="10"/>
+        <v>501010103</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>45</v>
+      </c>
+      <c r="B92" t="str">
+        <f t="shared" si="8"/>
+        <v>GRE for Pharmacy</v>
+      </c>
+      <c r="C92" t="s">
+        <v>33</v>
+      </c>
+      <c r="D92">
+        <v>5010102</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="10"/>
+        <v>501010201</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93" t="str">
+        <f t="shared" si="8"/>
+        <v>GRE for Pharmacy</v>
+      </c>
+      <c r="C93" t="s">
+        <v>33</v>
+      </c>
+      <c r="D93">
+        <v>5010102</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="10"/>
+        <v>501010202</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93" t="str">
+        <f>IF(F93&lt;&gt;1,"level5","form_field")</f>
+        <v>form_field</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>47</v>
+      </c>
+      <c r="B94" t="str">
+        <f t="shared" si="8"/>
+        <v>GRE for Pharmacy</v>
+      </c>
+      <c r="C94" t="s">
+        <v>33</v>
+      </c>
+      <c r="D94">
+        <v>5010102</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="10"/>
+        <v>501010203</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94" t="str">
+        <f t="shared" si="9"/>
+        <v>form_field</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="E95">
+        <f>IF(D95&lt;&gt;D94,((D95*100)+1),(E94+1))</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>